<commit_message>
Running at home, test at OA
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -387,7 +387,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="B9" pane="bottomLeft" sqref="B9"/>
+      <selection activeCell="A4" pane="bottomLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -395,7 +395,8 @@
     <col customWidth="1" max="1" min="1" style="1" width="52.85546875"/>
     <col customWidth="1" max="2" min="2" style="1" width="46.28515625"/>
     <col customWidth="1" max="3" min="3" style="1" width="40.85546875"/>
-    <col customWidth="1" max="16384" min="4" style="1" width="9.140625"/>
+    <col customWidth="1" max="7" min="4" style="1" width="9.140625"/>
+    <col customWidth="1" max="16384" min="8" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>